<commit_message>
Add toxic sewer; add new ut helm
</commit_message>
<xml_diff>
--- a/EquipmentStats.xlsx
+++ b/EquipmentStats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O677"/>
+  <dimension ref="A1:O684"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2916,7 +2916,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
@@ -2925,7 +2925,7 @@
         <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="K47" t="n">
         <v>0</v>
@@ -20839,7 +20839,7 @@
         <v>0</v>
       </c>
       <c r="J385" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K385" t="n">
         <v>0</v>
@@ -20851,7 +20851,7 @@
         <v>0</v>
       </c>
       <c r="N385" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O385" t="n">
         <v>0</v>
@@ -30721,24 +30721,24 @@
       </c>
       <c r="B572" t="inlineStr">
         <is>
-          <t>0xcd5</t>
+          <t>0xceb</t>
         </is>
       </c>
       <c r="C572" t="inlineStr">
         <is>
-          <t>Ivory Wyvern Key</t>
+          <t>Horned Suguyari</t>
         </is>
       </c>
       <c r="D572" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E572" t="n">
-        <v>0</v>
+        <v>360.5</v>
       </c>
       <c r="F572" t="n">
-        <v>0</v>
+        <v>324.45</v>
       </c>
       <c r="G572" t="n">
         <v>0</v>
@@ -30774,17 +30774,17 @@
       </c>
       <c r="B573" t="inlineStr">
         <is>
-          <t>0x6953</t>
+          <t>0xcec</t>
         </is>
       </c>
       <c r="C573" t="inlineStr">
         <is>
-          <t>Lost Halls Key</t>
+          <t>Seal of Havoc</t>
         </is>
       </c>
       <c r="D573" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E573" t="n">
@@ -30827,24 +30827,24 @@
       </c>
       <c r="B574" t="inlineStr">
         <is>
-          <t>0x024c</t>
+          <t>0xced</t>
         </is>
       </c>
       <c r="C574" t="inlineStr">
         <is>
-          <t>Bow of the Void</t>
+          <t>The Molten Cape</t>
         </is>
       </c>
       <c r="D574" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E574" t="n">
-        <v>257.5</v>
+        <v>0</v>
       </c>
       <c r="F574" t="n">
-        <v>321.875</v>
+        <v>0</v>
       </c>
       <c r="G574" t="n">
         <v>0</v>
@@ -30853,22 +30853,22 @@
         <v>0</v>
       </c>
       <c r="I574" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J574" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K574" t="n">
         <v>0</v>
       </c>
       <c r="L574" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M574" t="n">
         <v>0</v>
       </c>
       <c r="N574" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O574" t="n">
         <v>0</v>
@@ -30880,21 +30880,21 @@
       </c>
       <c r="B575" t="inlineStr">
         <is>
-          <t>0x024d</t>
+          <t>0xcee</t>
         </is>
       </c>
       <c r="C575" t="inlineStr">
         <is>
-          <t>Quiver of the Shadows</t>
+          <t>Scarlet's Power</t>
         </is>
       </c>
       <c r="D575" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E575" t="n">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="F575" t="n">
         <v>0</v>
@@ -30906,22 +30906,22 @@
         <v>0</v>
       </c>
       <c r="I575" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J575" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K575" t="n">
         <v>0</v>
       </c>
       <c r="L575" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M575" t="n">
         <v>0</v>
       </c>
       <c r="N575" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O575" t="n">
         <v>0</v>
@@ -30933,24 +30933,24 @@
       </c>
       <c r="B576" t="inlineStr">
         <is>
-          <t>0x024e</t>
+          <t>0xcef</t>
         </is>
       </c>
       <c r="C576" t="inlineStr">
         <is>
-          <t>Armor of Nil</t>
+          <t>Bow of War</t>
         </is>
       </c>
       <c r="D576" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E576" t="n">
-        <v>0</v>
+        <v>307.5</v>
       </c>
       <c r="F576" t="n">
-        <v>0</v>
+        <v>408.975</v>
       </c>
       <c r="G576" t="n">
         <v>0</v>
@@ -30959,13 +30959,13 @@
         <v>0</v>
       </c>
       <c r="I576" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J576" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="K576" t="n">
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="L576" t="n">
         <v>0</v>
@@ -30986,21 +30986,21 @@
       </c>
       <c r="B577" t="inlineStr">
         <is>
-          <t>0x024f</t>
+          <t>0xcd0</t>
         </is>
       </c>
       <c r="C577" t="inlineStr">
         <is>
-          <t>Sourcestone</t>
+          <t>The Red Shield</t>
         </is>
       </c>
       <c r="D577" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E577" t="n">
-        <v>0</v>
+        <v>217.5</v>
       </c>
       <c r="F577" t="n">
         <v>0</v>
@@ -31009,13 +31009,13 @@
         <v>0</v>
       </c>
       <c r="H577" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="I577" t="n">
         <v>0</v>
       </c>
       <c r="J577" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K577" t="n">
         <v>0</v>
@@ -31024,13 +31024,13 @@
         <v>0</v>
       </c>
       <c r="M577" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N577" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="O577" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="578">
@@ -31039,17 +31039,17 @@
       </c>
       <c r="B578" t="inlineStr">
         <is>
-          <t>0x0251</t>
+          <t>0xcd1</t>
         </is>
       </c>
       <c r="C578" t="inlineStr">
         <is>
-          <t>Omnipotence Ring</t>
+          <t>Rusted Helm</t>
         </is>
       </c>
       <c r="D578" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>16</t>
         </is>
       </c>
       <c r="E578" t="n">
@@ -31059,28 +31059,28 @@
         <v>0</v>
       </c>
       <c r="G578" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="H578" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="I578" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J578" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K578" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L578" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M578" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N578" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O578" t="n">
         <v>0</v>
@@ -31092,24 +31092,24 @@
       </c>
       <c r="B579" t="inlineStr">
         <is>
-          <t>0x0244</t>
+          <t>0xcd5</t>
         </is>
       </c>
       <c r="C579" t="inlineStr">
         <is>
-          <t>Staff of Unholy Sacrifice</t>
+          <t>Ivory Wyvern Key</t>
         </is>
       </c>
       <c r="D579" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E579" t="n">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="F579" t="n">
-        <v>585</v>
+        <v>0</v>
       </c>
       <c r="G579" t="n">
         <v>0</v>
@@ -31145,17 +31145,17 @@
       </c>
       <c r="B580" t="inlineStr">
         <is>
-          <t>0x0250</t>
+          <t>0x6953</t>
         </is>
       </c>
       <c r="C580" t="inlineStr">
         <is>
-          <t>Skull of Corrupted Souls</t>
+          <t>Lost Halls Key</t>
         </is>
       </c>
       <c r="D580" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E580" t="n">
@@ -31165,7 +31165,7 @@
         <v>0</v>
       </c>
       <c r="G580" t="n">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="H580" t="n">
         <v>0</v>
@@ -31183,7 +31183,7 @@
         <v>0</v>
       </c>
       <c r="M580" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N580" t="n">
         <v>0</v>
@@ -31198,36 +31198,36 @@
       </c>
       <c r="B581" t="inlineStr">
         <is>
-          <t>0x0252</t>
+          <t>0x024c</t>
         </is>
       </c>
       <c r="C581" t="inlineStr">
         <is>
-          <t>Ritual Robe</t>
+          <t>Bow of the Void</t>
         </is>
       </c>
       <c r="D581" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E581" t="n">
-        <v>0</v>
+        <v>257.5</v>
       </c>
       <c r="F581" t="n">
-        <v>0</v>
+        <v>321.875</v>
       </c>
       <c r="G581" t="n">
         <v>0</v>
       </c>
       <c r="H581" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="I581" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J581" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="K581" t="n">
         <v>0</v>
@@ -31239,7 +31239,7 @@
         <v>0</v>
       </c>
       <c r="N581" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="O581" t="n">
         <v>0</v>
@@ -31251,36 +31251,36 @@
       </c>
       <c r="B582" t="inlineStr">
         <is>
-          <t>0x0253</t>
+          <t>0x024d</t>
         </is>
       </c>
       <c r="C582" t="inlineStr">
         <is>
-          <t>Bloodshed Ring</t>
+          <t>Quiver of the Shadows</t>
         </is>
       </c>
       <c r="D582" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E582" t="n">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="F582" t="n">
         <v>0</v>
       </c>
       <c r="G582" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="H582" t="n">
         <v>0</v>
       </c>
       <c r="I582" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J582" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K582" t="n">
         <v>0</v>
@@ -31292,7 +31292,7 @@
         <v>0</v>
       </c>
       <c r="N582" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O582" t="n">
         <v>0</v>
@@ -31304,24 +31304,24 @@
       </c>
       <c r="B583" t="inlineStr">
         <is>
-          <t>0x0254</t>
+          <t>0x024e</t>
         </is>
       </c>
       <c r="C583" t="inlineStr">
         <is>
-          <t>Sword of the Colossus</t>
+          <t>Armor of Nil</t>
         </is>
       </c>
       <c r="D583" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E583" t="n">
-        <v>437.5</v>
+        <v>0</v>
       </c>
       <c r="F583" t="n">
-        <v>459.375</v>
+        <v>0</v>
       </c>
       <c r="G583" t="n">
         <v>0</v>
@@ -31330,13 +31330,13 @@
         <v>0</v>
       </c>
       <c r="I583" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J583" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="K583" t="n">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="L583" t="n">
         <v>0</v>
@@ -31357,17 +31357,17 @@
       </c>
       <c r="B584" t="inlineStr">
         <is>
-          <t>0x0243</t>
+          <t>0x024f</t>
         </is>
       </c>
       <c r="C584" t="inlineStr">
         <is>
-          <t>Marble Seal</t>
+          <t>Sourcestone</t>
         </is>
       </c>
       <c r="D584" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E584" t="n">
@@ -31380,13 +31380,13 @@
         <v>0</v>
       </c>
       <c r="H584" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="I584" t="n">
         <v>0</v>
       </c>
       <c r="J584" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K584" t="n">
         <v>0</v>
@@ -31398,7 +31398,7 @@
         <v>0</v>
       </c>
       <c r="N584" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O584" t="n">
         <v>0</v>
@@ -31410,17 +31410,17 @@
       </c>
       <c r="B585" t="inlineStr">
         <is>
-          <t>0x0255</t>
+          <t>0x0251</t>
         </is>
       </c>
       <c r="C585" t="inlineStr">
         <is>
-          <t>Breastplate of New Life</t>
+          <t>Omnipotence Ring</t>
         </is>
       </c>
       <c r="D585" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E585" t="n">
@@ -31430,28 +31430,28 @@
         <v>0</v>
       </c>
       <c r="G585" t="n">
-        <v>225</v>
+        <v>80</v>
       </c>
       <c r="H585" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="I585" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J585" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="K585" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L585" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M585" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N585" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O585" t="n">
         <v>0</v>
@@ -31463,24 +31463,24 @@
       </c>
       <c r="B586" t="inlineStr">
         <is>
-          <t>0x0256</t>
+          <t>0x0244</t>
         </is>
       </c>
       <c r="C586" t="inlineStr">
         <is>
-          <t>Magical Lodestone</t>
+          <t>Staff of Unholy Sacrifice</t>
         </is>
       </c>
       <c r="D586" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>17</t>
         </is>
       </c>
       <c r="E586" t="n">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="F586" t="n">
-        <v>0</v>
+        <v>585</v>
       </c>
       <c r="G586" t="n">
         <v>0</v>
@@ -31489,16 +31489,16 @@
         <v>0</v>
       </c>
       <c r="I586" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J586" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K586" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L586" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M586" t="n">
         <v>0</v>
@@ -31516,17 +31516,17 @@
       </c>
       <c r="B587" t="inlineStr">
         <is>
-          <t>0x0257</t>
+          <t>0x0250</t>
         </is>
       </c>
       <c r="C587" t="inlineStr">
         <is>
-          <t>Cloak of Bloody Surprises</t>
+          <t>Skull of Corrupted Souls</t>
         </is>
       </c>
       <c r="D587" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>19</t>
         </is>
       </c>
       <c r="E587" t="n">
@@ -31536,7 +31536,7 @@
         <v>0</v>
       </c>
       <c r="G587" t="n">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="H587" t="n">
         <v>0</v>
@@ -31545,7 +31545,7 @@
         <v>0</v>
       </c>
       <c r="J587" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K587" t="n">
         <v>0</v>
@@ -31554,7 +31554,7 @@
         <v>0</v>
       </c>
       <c r="M587" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="N587" t="n">
         <v>0</v>
@@ -31569,36 +31569,36 @@
       </c>
       <c r="B588" t="inlineStr">
         <is>
-          <t>0x0258</t>
+          <t>0x0252</t>
         </is>
       </c>
       <c r="C588" t="inlineStr">
         <is>
-          <t>Carved Golem Remains</t>
+          <t>Ritual Robe</t>
         </is>
       </c>
       <c r="D588" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E588" t="n">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="F588" t="n">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="G588" t="n">
         <v>0</v>
       </c>
       <c r="H588" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I588" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J588" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K588" t="n">
         <v>0</v>
@@ -31610,7 +31610,7 @@
         <v>0</v>
       </c>
       <c r="N588" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="O588" t="n">
         <v>0</v>
@@ -31622,33 +31622,33 @@
       </c>
       <c r="B589" t="inlineStr">
         <is>
-          <t>0x0259</t>
+          <t>0x0253</t>
         </is>
       </c>
       <c r="C589" t="inlineStr">
         <is>
-          <t>Brain of the Golem</t>
+          <t>Bloodshed Ring</t>
         </is>
       </c>
       <c r="D589" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E589" t="n">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="F589" t="n">
         <v>0</v>
       </c>
       <c r="G589" t="n">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="H589" t="n">
         <v>0</v>
       </c>
       <c r="I589" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J589" t="n">
         <v>0</v>
@@ -31663,7 +31663,7 @@
         <v>0</v>
       </c>
       <c r="N589" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O589" t="n">
         <v>0</v>
@@ -31675,24 +31675,24 @@
       </c>
       <c r="B590" t="inlineStr">
         <is>
-          <t>0x025a</t>
+          <t>0x0254</t>
         </is>
       </c>
       <c r="C590" t="inlineStr">
         <is>
-          <t>Golem Garments</t>
+          <t>Sword of the Colossus</t>
         </is>
       </c>
       <c r="D590" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E590" t="n">
-        <v>0</v>
+        <v>437.5</v>
       </c>
       <c r="F590" t="n">
-        <v>0</v>
+        <v>459.375</v>
       </c>
       <c r="G590" t="n">
         <v>0</v>
@@ -31701,10 +31701,10 @@
         <v>0</v>
       </c>
       <c r="I590" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J590" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="K590" t="n">
         <v>0</v>
@@ -31713,7 +31713,7 @@
         <v>0</v>
       </c>
       <c r="M590" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="N590" t="n">
         <v>0</v>
@@ -31728,17 +31728,17 @@
       </c>
       <c r="B591" t="inlineStr">
         <is>
-          <t>0x025b</t>
+          <t>0x0243</t>
         </is>
       </c>
       <c r="C591" t="inlineStr">
         <is>
-          <t>Rusty Cuffs</t>
+          <t>Marble Seal</t>
         </is>
       </c>
       <c r="D591" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E591" t="n">
@@ -31748,7 +31748,7 @@
         <v>0</v>
       </c>
       <c r="G591" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="H591" t="n">
         <v>0</v>
@@ -31760,7 +31760,7 @@
         <v>5</v>
       </c>
       <c r="K591" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L591" t="n">
         <v>0</v>
@@ -31781,17 +31781,17 @@
       </c>
       <c r="B592" t="inlineStr">
         <is>
-          <t>0x1500</t>
+          <t>0x0255</t>
         </is>
       </c>
       <c r="C592" t="inlineStr">
         <is>
-          <t>Black Cat Generator</t>
+          <t>Breastplate of New Life</t>
         </is>
       </c>
       <c r="D592" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E592" t="n">
@@ -31801,7 +31801,7 @@
         <v>0</v>
       </c>
       <c r="G592" t="n">
-        <v>0</v>
+        <v>225</v>
       </c>
       <c r="H592" t="n">
         <v>0</v>
@@ -31810,7 +31810,7 @@
         <v>0</v>
       </c>
       <c r="J592" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K592" t="n">
         <v>0</v>
@@ -31834,17 +31834,17 @@
       </c>
       <c r="B593" t="inlineStr">
         <is>
-          <t>0x1501</t>
+          <t>0x0256</t>
         </is>
       </c>
       <c r="C593" t="inlineStr">
         <is>
-          <t>Grey Cat Generator</t>
+          <t>Magical Lodestone</t>
         </is>
       </c>
       <c r="D593" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E593" t="n">
@@ -31860,16 +31860,16 @@
         <v>0</v>
       </c>
       <c r="I593" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J593" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K593" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L593" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M593" t="n">
         <v>0</v>
@@ -31887,17 +31887,17 @@
       </c>
       <c r="B594" t="inlineStr">
         <is>
-          <t>0x1502</t>
+          <t>0x0257</t>
         </is>
       </c>
       <c r="C594" t="inlineStr">
         <is>
-          <t>Orange Cat Generator</t>
+          <t>Cloak of Bloody Surprises</t>
         </is>
       </c>
       <c r="D594" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E594" t="n">
@@ -31916,7 +31916,7 @@
         <v>0</v>
       </c>
       <c r="J594" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K594" t="n">
         <v>0</v>
@@ -31925,7 +31925,7 @@
         <v>0</v>
       </c>
       <c r="M594" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N594" t="n">
         <v>0</v>
@@ -31940,24 +31940,24 @@
       </c>
       <c r="B595" t="inlineStr">
         <is>
-          <t>0x1503</t>
+          <t>0x0258</t>
         </is>
       </c>
       <c r="C595" t="inlineStr">
         <is>
-          <t>Tan Cat Generator</t>
+          <t>Carved Golem Remains</t>
         </is>
       </c>
       <c r="D595" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E595" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="F595" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="G595" t="n">
         <v>0</v>
@@ -31993,21 +31993,21 @@
       </c>
       <c r="B596" t="inlineStr">
         <is>
-          <t>0x1504</t>
+          <t>0x0259</t>
         </is>
       </c>
       <c r="C596" t="inlineStr">
         <is>
-          <t>Yellow Cat Generator</t>
+          <t>Brain of the Golem</t>
         </is>
       </c>
       <c r="D596" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>22</t>
         </is>
       </c>
       <c r="E596" t="n">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="F596" t="n">
         <v>0</v>
@@ -32046,17 +32046,17 @@
       </c>
       <c r="B597" t="inlineStr">
         <is>
-          <t>0x1505</t>
+          <t>0x025a</t>
         </is>
       </c>
       <c r="C597" t="inlineStr">
         <is>
-          <t>Brown Pup Generator</t>
+          <t>Golem Garments</t>
         </is>
       </c>
       <c r="D597" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E597" t="n">
@@ -32072,10 +32072,10 @@
         <v>0</v>
       </c>
       <c r="I597" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J597" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K597" t="n">
         <v>0</v>
@@ -32084,7 +32084,7 @@
         <v>0</v>
       </c>
       <c r="M597" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N597" t="n">
         <v>0</v>
@@ -32099,17 +32099,17 @@
       </c>
       <c r="B598" t="inlineStr">
         <is>
-          <t>0x1506</t>
+          <t>0x025b</t>
         </is>
       </c>
       <c r="C598" t="inlineStr">
         <is>
-          <t>Grey Pup Generator</t>
+          <t>Rusty Cuffs</t>
         </is>
       </c>
       <c r="D598" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E598" t="n">
@@ -32119,7 +32119,7 @@
         <v>0</v>
       </c>
       <c r="G598" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="H598" t="n">
         <v>0</v>
@@ -32128,10 +32128,10 @@
         <v>0</v>
       </c>
       <c r="J598" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K598" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L598" t="n">
         <v>0</v>
@@ -32152,12 +32152,12 @@
       </c>
       <c r="B599" t="inlineStr">
         <is>
-          <t>0x1507</t>
+          <t>0x1500</t>
         </is>
       </c>
       <c r="C599" t="inlineStr">
         <is>
-          <t>Golden Pup Generator</t>
+          <t>Black Cat Generator</t>
         </is>
       </c>
       <c r="D599" t="inlineStr">
@@ -32205,12 +32205,12 @@
       </c>
       <c r="B600" t="inlineStr">
         <is>
-          <t>0x1508</t>
+          <t>0x1501</t>
         </is>
       </c>
       <c r="C600" t="inlineStr">
         <is>
-          <t>White Cat Generator</t>
+          <t>Grey Cat Generator</t>
         </is>
       </c>
       <c r="D600" t="inlineStr">
@@ -32258,12 +32258,12 @@
       </c>
       <c r="B601" t="inlineStr">
         <is>
-          <t>0x1509</t>
+          <t>0x1502</t>
         </is>
       </c>
       <c r="C601" t="inlineStr">
         <is>
-          <t>Blue Snail Generator</t>
+          <t>Orange Cat Generator</t>
         </is>
       </c>
       <c r="D601" t="inlineStr">
@@ -32311,12 +32311,12 @@
       </c>
       <c r="B602" t="inlineStr">
         <is>
-          <t>0x150a</t>
+          <t>0x1503</t>
         </is>
       </c>
       <c r="C602" t="inlineStr">
         <is>
-          <t>Grey Wolf Generator</t>
+          <t>Tan Cat Generator</t>
         </is>
       </c>
       <c r="D602" t="inlineStr">
@@ -32364,12 +32364,12 @@
       </c>
       <c r="B603" t="inlineStr">
         <is>
-          <t>0x150b</t>
+          <t>0x1504</t>
         </is>
       </c>
       <c r="C603" t="inlineStr">
         <is>
-          <t>Brown Fox Generator</t>
+          <t>Yellow Cat Generator</t>
         </is>
       </c>
       <c r="D603" t="inlineStr">
@@ -32417,12 +32417,12 @@
       </c>
       <c r="B604" t="inlineStr">
         <is>
-          <t>0x150c</t>
+          <t>0x1505</t>
         </is>
       </c>
       <c r="C604" t="inlineStr">
         <is>
-          <t>Green Frog Generator</t>
+          <t>Brown Pup Generator</t>
         </is>
       </c>
       <c r="D604" t="inlineStr">
@@ -32470,12 +32470,12 @@
       </c>
       <c r="B605" t="inlineStr">
         <is>
-          <t>0x150d</t>
+          <t>0x1506</t>
         </is>
       </c>
       <c r="C605" t="inlineStr">
         <is>
-          <t>Lion Generator</t>
+          <t>Grey Pup Generator</t>
         </is>
       </c>
       <c r="D605" t="inlineStr">
@@ -32523,12 +32523,12 @@
       </c>
       <c r="B606" t="inlineStr">
         <is>
-          <t>0x150e</t>
+          <t>0x1507</t>
         </is>
       </c>
       <c r="C606" t="inlineStr">
         <is>
-          <t>Penguin Generator</t>
+          <t>Golden Pup Generator</t>
         </is>
       </c>
       <c r="D606" t="inlineStr">
@@ -32576,12 +32576,12 @@
       </c>
       <c r="B607" t="inlineStr">
         <is>
-          <t>0x150f</t>
+          <t>0x1508</t>
         </is>
       </c>
       <c r="C607" t="inlineStr">
         <is>
-          <t>Sheepdog Generator</t>
+          <t>White Cat Generator</t>
         </is>
       </c>
       <c r="D607" t="inlineStr">
@@ -32629,12 +32629,12 @@
       </c>
       <c r="B608" t="inlineStr">
         <is>
-          <t>0x1510</t>
+          <t>0x1509</t>
         </is>
       </c>
       <c r="C608" t="inlineStr">
         <is>
-          <t>Panda Generator</t>
+          <t>Blue Snail Generator</t>
         </is>
       </c>
       <c r="D608" t="inlineStr">
@@ -32682,12 +32682,12 @@
       </c>
       <c r="B609" t="inlineStr">
         <is>
-          <t>0x1511</t>
+          <t>0x150a</t>
         </is>
       </c>
       <c r="C609" t="inlineStr">
         <is>
-          <t>Purple Snail Generator</t>
+          <t>Grey Wolf Generator</t>
         </is>
       </c>
       <c r="D609" t="inlineStr">
@@ -32735,12 +32735,12 @@
       </c>
       <c r="B610" t="inlineStr">
         <is>
-          <t>0x1512</t>
+          <t>0x150b</t>
         </is>
       </c>
       <c r="C610" t="inlineStr">
         <is>
-          <t>Black Wolf Generator</t>
+          <t>Brown Fox Generator</t>
         </is>
       </c>
       <c r="D610" t="inlineStr">
@@ -32788,12 +32788,12 @@
       </c>
       <c r="B611" t="inlineStr">
         <is>
-          <t>0x1513</t>
+          <t>0x150c</t>
         </is>
       </c>
       <c r="C611" t="inlineStr">
         <is>
-          <t>Grey Fox Generator</t>
+          <t>Green Frog Generator</t>
         </is>
       </c>
       <c r="D611" t="inlineStr">
@@ -32841,12 +32841,12 @@
       </c>
       <c r="B612" t="inlineStr">
         <is>
-          <t>0x1514</t>
+          <t>0x150d</t>
         </is>
       </c>
       <c r="C612" t="inlineStr">
         <is>
-          <t>Purple Frog Generator</t>
+          <t>Lion Generator</t>
         </is>
       </c>
       <c r="D612" t="inlineStr">
@@ -32894,12 +32894,12 @@
       </c>
       <c r="B613" t="inlineStr">
         <is>
-          <t>0x1515</t>
+          <t>0x150e</t>
         </is>
       </c>
       <c r="C613" t="inlineStr">
         <is>
-          <t>White Lion Generator</t>
+          <t>Penguin Generator</t>
         </is>
       </c>
       <c r="D613" t="inlineStr">
@@ -32947,12 +32947,12 @@
       </c>
       <c r="B614" t="inlineStr">
         <is>
-          <t>0x1516</t>
+          <t>0x150f</t>
         </is>
       </c>
       <c r="C614" t="inlineStr">
         <is>
-          <t>Green Penguin Generator</t>
+          <t>Sheepdog Generator</t>
         </is>
       </c>
       <c r="D614" t="inlineStr">
@@ -33000,12 +33000,12 @@
       </c>
       <c r="B615" t="inlineStr">
         <is>
-          <t>0x1517</t>
+          <t>0x1510</t>
         </is>
       </c>
       <c r="C615" t="inlineStr">
         <is>
-          <t>Golden Sheepdog Generator</t>
+          <t>Panda Generator</t>
         </is>
       </c>
       <c r="D615" t="inlineStr">
@@ -33053,12 +33053,12 @@
       </c>
       <c r="B616" t="inlineStr">
         <is>
-          <t>0x1518</t>
+          <t>0x1511</t>
         </is>
       </c>
       <c r="C616" t="inlineStr">
         <is>
-          <t>Bluebird Generator</t>
+          <t>Purple Snail Generator</t>
         </is>
       </c>
       <c r="D616" t="inlineStr">
@@ -33106,12 +33106,12 @@
       </c>
       <c r="B617" t="inlineStr">
         <is>
-          <t>0x1519</t>
+          <t>0x1512</t>
         </is>
       </c>
       <c r="C617" t="inlineStr">
         <is>
-          <t>Chick Generator</t>
+          <t>Black Wolf Generator</t>
         </is>
       </c>
       <c r="D617" t="inlineStr">
@@ -33159,12 +33159,12 @@
       </c>
       <c r="B618" t="inlineStr">
         <is>
-          <t>0x151a</t>
+          <t>0x1513</t>
         </is>
       </c>
       <c r="C618" t="inlineStr">
         <is>
-          <t>Pig Generator</t>
+          <t>Grey Fox Generator</t>
         </is>
       </c>
       <c r="D618" t="inlineStr">
@@ -33212,12 +33212,12 @@
       </c>
       <c r="B619" t="inlineStr">
         <is>
-          <t>0x151b</t>
+          <t>0x1514</t>
         </is>
       </c>
       <c r="C619" t="inlineStr">
         <is>
-          <t>Sea Slurp Generator</t>
+          <t>Purple Frog Generator</t>
         </is>
       </c>
       <c r="D619" t="inlineStr">
@@ -33265,12 +33265,12 @@
       </c>
       <c r="B620" t="inlineStr">
         <is>
-          <t>0x151c</t>
+          <t>0x1515</t>
         </is>
       </c>
       <c r="C620" t="inlineStr">
         <is>
-          <t>Squirrel Generator</t>
+          <t>White Lion Generator</t>
         </is>
       </c>
       <c r="D620" t="inlineStr">
@@ -33318,12 +33318,12 @@
       </c>
       <c r="B621" t="inlineStr">
         <is>
-          <t>0x151d</t>
+          <t>0x1516</t>
         </is>
       </c>
       <c r="C621" t="inlineStr">
         <is>
-          <t>Bat Generator</t>
+          <t>Green Penguin Generator</t>
         </is>
       </c>
       <c r="D621" t="inlineStr">
@@ -33371,12 +33371,12 @@
       </c>
       <c r="B622" t="inlineStr">
         <is>
-          <t>0x151e</t>
+          <t>0x1517</t>
         </is>
       </c>
       <c r="C622" t="inlineStr">
         <is>
-          <t>Lil' Ghost Generator</t>
+          <t>Golden Sheepdog Generator</t>
         </is>
       </c>
       <c r="D622" t="inlineStr">
@@ -33424,12 +33424,12 @@
       </c>
       <c r="B623" t="inlineStr">
         <is>
-          <t>0x151f</t>
+          <t>0x1518</t>
         </is>
       </c>
       <c r="C623" t="inlineStr">
         <is>
-          <t>Valentine Generator</t>
+          <t>Bluebird Generator</t>
         </is>
       </c>
       <c r="D623" t="inlineStr">
@@ -33477,12 +33477,12 @@
       </c>
       <c r="B624" t="inlineStr">
         <is>
-          <t>0x1520</t>
+          <t>0x1519</t>
         </is>
       </c>
       <c r="C624" t="inlineStr">
         <is>
-          <t>Leprechaun Generator</t>
+          <t>Chick Generator</t>
         </is>
       </c>
       <c r="D624" t="inlineStr">
@@ -33530,12 +33530,12 @@
       </c>
       <c r="B625" t="inlineStr">
         <is>
-          <t>0x1521</t>
+          <t>0x151a</t>
         </is>
       </c>
       <c r="C625" t="inlineStr">
         <is>
-          <t>Lil' Oryx Generator</t>
+          <t>Pig Generator</t>
         </is>
       </c>
       <c r="D625" t="inlineStr">
@@ -33583,12 +33583,12 @@
       </c>
       <c r="B626" t="inlineStr">
         <is>
-          <t>0x1522</t>
+          <t>0x151b</t>
         </is>
       </c>
       <c r="C626" t="inlineStr">
         <is>
-          <t>Toucan Generator</t>
+          <t>Sea Slurp Generator</t>
         </is>
       </c>
       <c r="D626" t="inlineStr">
@@ -33636,12 +33636,12 @@
       </c>
       <c r="B627" t="inlineStr">
         <is>
-          <t>0x1523</t>
+          <t>0x151c</t>
         </is>
       </c>
       <c r="C627" t="inlineStr">
         <is>
-          <t>Skunk Generator</t>
+          <t>Squirrel Generator</t>
         </is>
       </c>
       <c r="D627" t="inlineStr">
@@ -33689,12 +33689,12 @@
       </c>
       <c r="B628" t="inlineStr">
         <is>
-          <t>0x1524</t>
+          <t>0x151d</t>
         </is>
       </c>
       <c r="C628" t="inlineStr">
         <is>
-          <t>Mallard Generator</t>
+          <t>Bat Generator</t>
         </is>
       </c>
       <c r="D628" t="inlineStr">
@@ -33742,12 +33742,12 @@
       </c>
       <c r="B629" t="inlineStr">
         <is>
-          <t>0x1525</t>
+          <t>0x151e</t>
         </is>
       </c>
       <c r="C629" t="inlineStr">
         <is>
-          <t>Duck Generator</t>
+          <t>Lil' Ghost Generator</t>
         </is>
       </c>
       <c r="D629" t="inlineStr">
@@ -33795,12 +33795,12 @@
       </c>
       <c r="B630" t="inlineStr">
         <is>
-          <t>0x1526</t>
+          <t>0x151f</t>
         </is>
       </c>
       <c r="C630" t="inlineStr">
         <is>
-          <t>Eagle Generator</t>
+          <t>Valentine Generator</t>
         </is>
       </c>
       <c r="D630" t="inlineStr">
@@ -33848,12 +33848,12 @@
       </c>
       <c r="B631" t="inlineStr">
         <is>
-          <t>0x1527</t>
+          <t>0x1520</t>
         </is>
       </c>
       <c r="C631" t="inlineStr">
         <is>
-          <t>Turtle Generator</t>
+          <t>Leprechaun Generator</t>
         </is>
       </c>
       <c r="D631" t="inlineStr">
@@ -33901,12 +33901,12 @@
       </c>
       <c r="B632" t="inlineStr">
         <is>
-          <t>0x1528</t>
+          <t>0x1521</t>
         </is>
       </c>
       <c r="C632" t="inlineStr">
         <is>
-          <t>Jelly Generator</t>
+          <t>Lil' Oryx Generator</t>
         </is>
       </c>
       <c r="D632" t="inlineStr">
@@ -33954,12 +33954,12 @@
       </c>
       <c r="B633" t="inlineStr">
         <is>
-          <t>0x1529</t>
+          <t>0x1522</t>
         </is>
       </c>
       <c r="C633" t="inlineStr">
         <is>
-          <t>Bee Generator</t>
+          <t>Toucan Generator</t>
         </is>
       </c>
       <c r="D633" t="inlineStr">
@@ -34007,12 +34007,12 @@
       </c>
       <c r="B634" t="inlineStr">
         <is>
-          <t>0x152a</t>
+          <t>0x1523</t>
         </is>
       </c>
       <c r="C634" t="inlineStr">
         <is>
-          <t>Raven Generator</t>
+          <t>Skunk Generator</t>
         </is>
       </c>
       <c r="D634" t="inlineStr">
@@ -34060,12 +34060,12 @@
       </c>
       <c r="B635" t="inlineStr">
         <is>
-          <t>0x152b</t>
+          <t>0x1524</t>
         </is>
       </c>
       <c r="C635" t="inlineStr">
         <is>
-          <t>Purple Penguin Generator</t>
+          <t>Mallard Generator</t>
         </is>
       </c>
       <c r="D635" t="inlineStr">
@@ -34113,12 +34113,12 @@
       </c>
       <c r="B636" t="inlineStr">
         <is>
-          <t>0x152c</t>
+          <t>0x1525</t>
         </is>
       </c>
       <c r="C636" t="inlineStr">
         <is>
-          <t>Grass Penguin Generator</t>
+          <t>Duck Generator</t>
         </is>
       </c>
       <c r="D636" t="inlineStr">
@@ -34166,12 +34166,12 @@
       </c>
       <c r="B637" t="inlineStr">
         <is>
-          <t>0x152d</t>
+          <t>0x1526</t>
         </is>
       </c>
       <c r="C637" t="inlineStr">
         <is>
-          <t>Elf Generator</t>
+          <t>Eagle Generator</t>
         </is>
       </c>
       <c r="D637" t="inlineStr">
@@ -34219,12 +34219,12 @@
       </c>
       <c r="B638" t="inlineStr">
         <is>
-          <t>0x152e</t>
+          <t>0x1527</t>
         </is>
       </c>
       <c r="C638" t="inlineStr">
         <is>
-          <t>Crab Generator</t>
+          <t>Turtle Generator</t>
         </is>
       </c>
       <c r="D638" t="inlineStr">
@@ -34272,12 +34272,12 @@
       </c>
       <c r="B639" t="inlineStr">
         <is>
-          <t>0x152f</t>
+          <t>0x1528</t>
         </is>
       </c>
       <c r="C639" t="inlineStr">
         <is>
-          <t>Hamster Generator</t>
+          <t>Jelly Generator</t>
         </is>
       </c>
       <c r="D639" t="inlineStr">
@@ -34325,12 +34325,12 @@
       </c>
       <c r="B640" t="inlineStr">
         <is>
-          <t>0x1530</t>
+          <t>0x1529</t>
         </is>
       </c>
       <c r="C640" t="inlineStr">
         <is>
-          <t>Dino Generator</t>
+          <t>Bee Generator</t>
         </is>
       </c>
       <c r="D640" t="inlineStr">
@@ -34378,12 +34378,12 @@
       </c>
       <c r="B641" t="inlineStr">
         <is>
-          <t>0x1531</t>
+          <t>0x152a</t>
         </is>
       </c>
       <c r="C641" t="inlineStr">
         <is>
-          <t>Elephant Generator</t>
+          <t>Raven Generator</t>
         </is>
       </c>
       <c r="D641" t="inlineStr">
@@ -34431,12 +34431,12 @@
       </c>
       <c r="B642" t="inlineStr">
         <is>
-          <t>0x1532</t>
+          <t>0x152b</t>
         </is>
       </c>
       <c r="C642" t="inlineStr">
         <is>
-          <t>Demon Frog Generator</t>
+          <t>Purple Penguin Generator</t>
         </is>
       </c>
       <c r="D642" t="inlineStr">
@@ -34484,12 +34484,12 @@
       </c>
       <c r="B643" t="inlineStr">
         <is>
-          <t>0x1533</t>
+          <t>0x152c</t>
         </is>
       </c>
       <c r="C643" t="inlineStr">
         <is>
-          <t>Gargoyle Generator</t>
+          <t>Grass Penguin Generator</t>
         </is>
       </c>
       <c r="D643" t="inlineStr">
@@ -34537,12 +34537,12 @@
       </c>
       <c r="B644" t="inlineStr">
         <is>
-          <t>0x1534</t>
+          <t>0x152d</t>
         </is>
       </c>
       <c r="C644" t="inlineStr">
         <is>
-          <t>Gummy Bear Generator</t>
+          <t>Elf Generator</t>
         </is>
       </c>
       <c r="D644" t="inlineStr">
@@ -34590,12 +34590,12 @@
       </c>
       <c r="B645" t="inlineStr">
         <is>
-          <t>0x1535</t>
+          <t>0x152e</t>
         </is>
       </c>
       <c r="C645" t="inlineStr">
         <is>
-          <t>Dragonfly Generator</t>
+          <t>Crab Generator</t>
         </is>
       </c>
       <c r="D645" t="inlineStr">
@@ -34643,12 +34643,12 @@
       </c>
       <c r="B646" t="inlineStr">
         <is>
-          <t>0x1536</t>
+          <t>0x152f</t>
         </is>
       </c>
       <c r="C646" t="inlineStr">
         <is>
-          <t>Lil' Cyclops Generator</t>
+          <t>Hamster Generator</t>
         </is>
       </c>
       <c r="D646" t="inlineStr">
@@ -34696,12 +34696,12 @@
       </c>
       <c r="B647" t="inlineStr">
         <is>
-          <t>0x1537</t>
+          <t>0x1530</t>
         </is>
       </c>
       <c r="C647" t="inlineStr">
         <is>
-          <t>Snowy Owl Generator</t>
+          <t>Dino Generator</t>
         </is>
       </c>
       <c r="D647" t="inlineStr">
@@ -34749,12 +34749,12 @@
       </c>
       <c r="B648" t="inlineStr">
         <is>
-          <t>0x1538</t>
+          <t>0x1531</t>
         </is>
       </c>
       <c r="C648" t="inlineStr">
         <is>
-          <t>Turkey Generator</t>
+          <t>Elephant Generator</t>
         </is>
       </c>
       <c r="D648" t="inlineStr">
@@ -34802,12 +34802,12 @@
       </c>
       <c r="B649" t="inlineStr">
         <is>
-          <t>0x1539</t>
+          <t>0x1532</t>
         </is>
       </c>
       <c r="C649" t="inlineStr">
         <is>
-          <t>Baby Generator</t>
+          <t>Demon Frog Generator</t>
         </is>
       </c>
       <c r="D649" t="inlineStr">
@@ -34855,12 +34855,12 @@
       </c>
       <c r="B650" t="inlineStr">
         <is>
-          <t>0x153a</t>
+          <t>0x1533</t>
         </is>
       </c>
       <c r="C650" t="inlineStr">
         <is>
-          <t>Baby Dragon Generator</t>
+          <t>Gargoyle Generator</t>
         </is>
       </c>
       <c r="D650" t="inlineStr">
@@ -34908,12 +34908,12 @@
       </c>
       <c r="B651" t="inlineStr">
         <is>
-          <t>0x153b</t>
+          <t>0x1534</t>
         </is>
       </c>
       <c r="C651" t="inlineStr">
         <is>
-          <t>Karate Penguin Red Generator</t>
+          <t>Gummy Bear Generator</t>
         </is>
       </c>
       <c r="D651" t="inlineStr">
@@ -34961,12 +34961,12 @@
       </c>
       <c r="B652" t="inlineStr">
         <is>
-          <t>0x153c</t>
+          <t>0x1535</t>
         </is>
       </c>
       <c r="C652" t="inlineStr">
         <is>
-          <t>Karate Penguin Blue Generator</t>
+          <t>Dragonfly Generator</t>
         </is>
       </c>
       <c r="D652" t="inlineStr">
@@ -35014,12 +35014,12 @@
       </c>
       <c r="B653" t="inlineStr">
         <is>
-          <t>0x153d</t>
+          <t>0x1536</t>
         </is>
       </c>
       <c r="C653" t="inlineStr">
         <is>
-          <t>Karate Penguin Yellow Generator</t>
+          <t>Lil' Cyclops Generator</t>
         </is>
       </c>
       <c r="D653" t="inlineStr">
@@ -35067,12 +35067,12 @@
       </c>
       <c r="B654" t="inlineStr">
         <is>
-          <t>0x153e</t>
+          <t>0x1537</t>
         </is>
       </c>
       <c r="C654" t="inlineStr">
         <is>
-          <t>Karate Penguin Purple Generator</t>
+          <t>Snowy Owl Generator</t>
         </is>
       </c>
       <c r="D654" t="inlineStr">
@@ -35120,12 +35120,12 @@
       </c>
       <c r="B655" t="inlineStr">
         <is>
-          <t>0x153f</t>
+          <t>0x1538</t>
         </is>
       </c>
       <c r="C655" t="inlineStr">
         <is>
-          <t>Beach Ball Generator</t>
+          <t>Turkey Generator</t>
         </is>
       </c>
       <c r="D655" t="inlineStr">
@@ -35173,12 +35173,12 @@
       </c>
       <c r="B656" t="inlineStr">
         <is>
-          <t>0x1540</t>
+          <t>0x1539</t>
         </is>
       </c>
       <c r="C656" t="inlineStr">
         <is>
-          <t>Robobuddy Generator</t>
+          <t>Baby Generator</t>
         </is>
       </c>
       <c r="D656" t="inlineStr">
@@ -35226,12 +35226,12 @@
       </c>
       <c r="B657" t="inlineStr">
         <is>
-          <t>0x1541</t>
+          <t>0x153a</t>
         </is>
       </c>
       <c r="C657" t="inlineStr">
         <is>
-          <t>Snowman Generator</t>
+          <t>Baby Dragon Generator</t>
         </is>
       </c>
       <c r="D657" t="inlineStr">
@@ -35279,12 +35279,12 @@
       </c>
       <c r="B658" t="inlineStr">
         <is>
-          <t>0x1542</t>
+          <t>0x153b</t>
         </is>
       </c>
       <c r="C658" t="inlineStr">
         <is>
-          <t>Black Ant Generator</t>
+          <t>Karate Penguin Red Generator</t>
         </is>
       </c>
       <c r="D658" t="inlineStr">
@@ -35332,12 +35332,12 @@
       </c>
       <c r="B659" t="inlineStr">
         <is>
-          <t>0x1543</t>
+          <t>0x153c</t>
         </is>
       </c>
       <c r="C659" t="inlineStr">
         <is>
-          <t>Blue Ant Generator</t>
+          <t>Karate Penguin Blue Generator</t>
         </is>
       </c>
       <c r="D659" t="inlineStr">
@@ -35385,12 +35385,12 @@
       </c>
       <c r="B660" t="inlineStr">
         <is>
-          <t>0x1544</t>
+          <t>0x153d</t>
         </is>
       </c>
       <c r="C660" t="inlineStr">
         <is>
-          <t>Green Ant Generator</t>
+          <t>Karate Penguin Yellow Generator</t>
         </is>
       </c>
       <c r="D660" t="inlineStr">
@@ -35438,12 +35438,12 @@
       </c>
       <c r="B661" t="inlineStr">
         <is>
-          <t>0x1545</t>
+          <t>0x153e</t>
         </is>
       </c>
       <c r="C661" t="inlineStr">
         <is>
-          <t>Red Ant Generator</t>
+          <t>Karate Penguin Purple Generator</t>
         </is>
       </c>
       <c r="D661" t="inlineStr">
@@ -35491,12 +35491,12 @@
       </c>
       <c r="B662" t="inlineStr">
         <is>
-          <t>0x1546</t>
+          <t>0x153f</t>
         </is>
       </c>
       <c r="C662" t="inlineStr">
         <is>
-          <t>Purple Ant Generator</t>
+          <t>Beach Ball Generator</t>
         </is>
       </c>
       <c r="D662" t="inlineStr">
@@ -35544,12 +35544,12 @@
       </c>
       <c r="B663" t="inlineStr">
         <is>
-          <t>0x1547</t>
+          <t>0x1540</t>
         </is>
       </c>
       <c r="C663" t="inlineStr">
         <is>
-          <t>Beer Slurp Generator</t>
+          <t>Robobuddy Generator</t>
         </is>
       </c>
       <c r="D663" t="inlineStr">
@@ -35597,12 +35597,12 @@
       </c>
       <c r="B664" t="inlineStr">
         <is>
-          <t>0x15aa</t>
+          <t>0x1541</t>
         </is>
       </c>
       <c r="C664" t="inlineStr">
         <is>
-          <t>Ball Generator</t>
+          <t>Snowman Generator</t>
         </is>
       </c>
       <c r="D664" t="inlineStr">
@@ -35650,12 +35650,12 @@
       </c>
       <c r="B665" t="inlineStr">
         <is>
-          <t>0x1549</t>
+          <t>0x1542</t>
         </is>
       </c>
       <c r="C665" t="inlineStr">
         <is>
-          <t>Peppermint Snail Generator</t>
+          <t>Black Ant Generator</t>
         </is>
       </c>
       <c r="D665" t="inlineStr">
@@ -35703,12 +35703,12 @@
       </c>
       <c r="B666" t="inlineStr">
         <is>
-          <t>0x154a</t>
+          <t>0x1543</t>
         </is>
       </c>
       <c r="C666" t="inlineStr">
         <is>
-          <t>Relief Oriole Generator</t>
+          <t>Blue Ant Generator</t>
         </is>
       </c>
       <c r="D666" t="inlineStr">
@@ -35756,12 +35756,12 @@
       </c>
       <c r="B667" t="inlineStr">
         <is>
-          <t>0x154b</t>
+          <t>0x1544</t>
         </is>
       </c>
       <c r="C667" t="inlineStr">
         <is>
-          <t>Relief Goldfinch Generator</t>
+          <t>Green Ant Generator</t>
         </is>
       </c>
       <c r="D667" t="inlineStr">
@@ -35809,12 +35809,12 @@
       </c>
       <c r="B668" t="inlineStr">
         <is>
-          <t>0x154c</t>
+          <t>0x1545</t>
         </is>
       </c>
       <c r="C668" t="inlineStr">
         <is>
-          <t>Relief Bluebird Generator</t>
+          <t>Red Ant Generator</t>
         </is>
       </c>
       <c r="D668" t="inlineStr">
@@ -35862,12 +35862,12 @@
       </c>
       <c r="B669" t="inlineStr">
         <is>
-          <t>0x154d</t>
+          <t>0x1546</t>
         </is>
       </c>
       <c r="C669" t="inlineStr">
         <is>
-          <t>Relief Cardinal Generator</t>
+          <t>Purple Ant Generator</t>
         </is>
       </c>
       <c r="D669" t="inlineStr">
@@ -35915,12 +35915,12 @@
       </c>
       <c r="B670" t="inlineStr">
         <is>
-          <t>0x154e</t>
+          <t>0x1547</t>
         </is>
       </c>
       <c r="C670" t="inlineStr">
         <is>
-          <t>Tamed Werewolf Cub Generator</t>
+          <t>Beer Slurp Generator</t>
         </is>
       </c>
       <c r="D670" t="inlineStr">
@@ -35968,12 +35968,12 @@
       </c>
       <c r="B671" t="inlineStr">
         <is>
-          <t>0x154f</t>
+          <t>0x15aa</t>
         </is>
       </c>
       <c r="C671" t="inlineStr">
         <is>
-          <t>Tomb Snake Generator</t>
+          <t>Ball Generator</t>
         </is>
       </c>
       <c r="D671" t="inlineStr">
@@ -36021,12 +36021,12 @@
       </c>
       <c r="B672" t="inlineStr">
         <is>
-          <t>0x1550</t>
+          <t>0x1549</t>
         </is>
       </c>
       <c r="C672" t="inlineStr">
         <is>
-          <t>Ninja Cat Generator</t>
+          <t>Peppermint Snail Generator</t>
         </is>
       </c>
       <c r="D672" t="inlineStr">
@@ -36074,12 +36074,12 @@
       </c>
       <c r="B673" t="inlineStr">
         <is>
-          <t>0x1551</t>
+          <t>0x154a</t>
         </is>
       </c>
       <c r="C673" t="inlineStr">
         <is>
-          <t>Praying Mantis Generator</t>
+          <t>Relief Oriole Generator</t>
         </is>
       </c>
       <c r="D673" t="inlineStr">
@@ -36127,12 +36127,12 @@
       </c>
       <c r="B674" t="inlineStr">
         <is>
-          <t>0x1552</t>
+          <t>0x154b</t>
         </is>
       </c>
       <c r="C674" t="inlineStr">
         <is>
-          <t>Dreidel Generator</t>
+          <t>Relief Goldfinch Generator</t>
         </is>
       </c>
       <c r="D674" t="inlineStr">
@@ -36180,12 +36180,12 @@
       </c>
       <c r="B675" t="inlineStr">
         <is>
-          <t>0x1654</t>
+          <t>0x154c</t>
         </is>
       </c>
       <c r="C675" t="inlineStr">
         <is>
-          <t>Witch Generator</t>
+          <t>Relief Bluebird Generator</t>
         </is>
       </c>
       <c r="D675" t="inlineStr">
@@ -36233,12 +36233,12 @@
       </c>
       <c r="B676" t="inlineStr">
         <is>
-          <t>0x1656</t>
+          <t>0x154d</t>
         </is>
       </c>
       <c r="C676" t="inlineStr">
         <is>
-          <t>Spider Generator</t>
+          <t>Relief Cardinal Generator</t>
         </is>
       </c>
       <c r="D676" t="inlineStr">
@@ -36286,50 +36286,421 @@
       </c>
       <c r="B677" t="inlineStr">
         <is>
+          <t>0x154e</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>Tamed Werewolf Cub Generator</t>
+        </is>
+      </c>
+      <c r="D677" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E677" t="n">
+        <v>0</v>
+      </c>
+      <c r="F677" t="n">
+        <v>0</v>
+      </c>
+      <c r="G677" t="n">
+        <v>0</v>
+      </c>
+      <c r="H677" t="n">
+        <v>0</v>
+      </c>
+      <c r="I677" t="n">
+        <v>0</v>
+      </c>
+      <c r="J677" t="n">
+        <v>0</v>
+      </c>
+      <c r="K677" t="n">
+        <v>0</v>
+      </c>
+      <c r="L677" t="n">
+        <v>0</v>
+      </c>
+      <c r="M677" t="n">
+        <v>0</v>
+      </c>
+      <c r="N677" t="n">
+        <v>0</v>
+      </c>
+      <c r="O677" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" s="1" t="n">
+        <v>676</v>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>0x154f</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>Tomb Snake Generator</t>
+        </is>
+      </c>
+      <c r="D678" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E678" t="n">
+        <v>0</v>
+      </c>
+      <c r="F678" t="n">
+        <v>0</v>
+      </c>
+      <c r="G678" t="n">
+        <v>0</v>
+      </c>
+      <c r="H678" t="n">
+        <v>0</v>
+      </c>
+      <c r="I678" t="n">
+        <v>0</v>
+      </c>
+      <c r="J678" t="n">
+        <v>0</v>
+      </c>
+      <c r="K678" t="n">
+        <v>0</v>
+      </c>
+      <c r="L678" t="n">
+        <v>0</v>
+      </c>
+      <c r="M678" t="n">
+        <v>0</v>
+      </c>
+      <c r="N678" t="n">
+        <v>0</v>
+      </c>
+      <c r="O678" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" s="1" t="n">
+        <v>677</v>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>0x1550</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>Ninja Cat Generator</t>
+        </is>
+      </c>
+      <c r="D679" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E679" t="n">
+        <v>0</v>
+      </c>
+      <c r="F679" t="n">
+        <v>0</v>
+      </c>
+      <c r="G679" t="n">
+        <v>0</v>
+      </c>
+      <c r="H679" t="n">
+        <v>0</v>
+      </c>
+      <c r="I679" t="n">
+        <v>0</v>
+      </c>
+      <c r="J679" t="n">
+        <v>0</v>
+      </c>
+      <c r="K679" t="n">
+        <v>0</v>
+      </c>
+      <c r="L679" t="n">
+        <v>0</v>
+      </c>
+      <c r="M679" t="n">
+        <v>0</v>
+      </c>
+      <c r="N679" t="n">
+        <v>0</v>
+      </c>
+      <c r="O679" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" s="1" t="n">
+        <v>678</v>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>0x1551</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>Praying Mantis Generator</t>
+        </is>
+      </c>
+      <c r="D680" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E680" t="n">
+        <v>0</v>
+      </c>
+      <c r="F680" t="n">
+        <v>0</v>
+      </c>
+      <c r="G680" t="n">
+        <v>0</v>
+      </c>
+      <c r="H680" t="n">
+        <v>0</v>
+      </c>
+      <c r="I680" t="n">
+        <v>0</v>
+      </c>
+      <c r="J680" t="n">
+        <v>0</v>
+      </c>
+      <c r="K680" t="n">
+        <v>0</v>
+      </c>
+      <c r="L680" t="n">
+        <v>0</v>
+      </c>
+      <c r="M680" t="n">
+        <v>0</v>
+      </c>
+      <c r="N680" t="n">
+        <v>0</v>
+      </c>
+      <c r="O680" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" s="1" t="n">
+        <v>679</v>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>0x1552</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>Dreidel Generator</t>
+        </is>
+      </c>
+      <c r="D681" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E681" t="n">
+        <v>0</v>
+      </c>
+      <c r="F681" t="n">
+        <v>0</v>
+      </c>
+      <c r="G681" t="n">
+        <v>0</v>
+      </c>
+      <c r="H681" t="n">
+        <v>0</v>
+      </c>
+      <c r="I681" t="n">
+        <v>0</v>
+      </c>
+      <c r="J681" t="n">
+        <v>0</v>
+      </c>
+      <c r="K681" t="n">
+        <v>0</v>
+      </c>
+      <c r="L681" t="n">
+        <v>0</v>
+      </c>
+      <c r="M681" t="n">
+        <v>0</v>
+      </c>
+      <c r="N681" t="n">
+        <v>0</v>
+      </c>
+      <c r="O681" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" s="1" t="n">
+        <v>680</v>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>0x1654</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>Witch Generator</t>
+        </is>
+      </c>
+      <c r="D682" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E682" t="n">
+        <v>0</v>
+      </c>
+      <c r="F682" t="n">
+        <v>0</v>
+      </c>
+      <c r="G682" t="n">
+        <v>0</v>
+      </c>
+      <c r="H682" t="n">
+        <v>0</v>
+      </c>
+      <c r="I682" t="n">
+        <v>0</v>
+      </c>
+      <c r="J682" t="n">
+        <v>0</v>
+      </c>
+      <c r="K682" t="n">
+        <v>0</v>
+      </c>
+      <c r="L682" t="n">
+        <v>0</v>
+      </c>
+      <c r="M682" t="n">
+        <v>0</v>
+      </c>
+      <c r="N682" t="n">
+        <v>0</v>
+      </c>
+      <c r="O682" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" s="1" t="n">
+        <v>681</v>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>0x1656</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>Spider Generator</t>
+        </is>
+      </c>
+      <c r="D683" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E683" t="n">
+        <v>0</v>
+      </c>
+      <c r="F683" t="n">
+        <v>0</v>
+      </c>
+      <c r="G683" t="n">
+        <v>0</v>
+      </c>
+      <c r="H683" t="n">
+        <v>0</v>
+      </c>
+      <c r="I683" t="n">
+        <v>0</v>
+      </c>
+      <c r="J683" t="n">
+        <v>0</v>
+      </c>
+      <c r="K683" t="n">
+        <v>0</v>
+      </c>
+      <c r="L683" t="n">
+        <v>0</v>
+      </c>
+      <c r="M683" t="n">
+        <v>0</v>
+      </c>
+      <c r="N683" t="n">
+        <v>0</v>
+      </c>
+      <c r="O683" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" s="1" t="n">
+        <v>682</v>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
           <t>0x1658</t>
         </is>
       </c>
-      <c r="C677" t="inlineStr">
+      <c r="C684" t="inlineStr">
         <is>
           <t>Sumo Generator</t>
         </is>
       </c>
-      <c r="D677" t="inlineStr">
+      <c r="D684" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="E677" t="n">
-        <v>0</v>
-      </c>
-      <c r="F677" t="n">
-        <v>0</v>
-      </c>
-      <c r="G677" t="n">
-        <v>0</v>
-      </c>
-      <c r="H677" t="n">
-        <v>0</v>
-      </c>
-      <c r="I677" t="n">
-        <v>0</v>
-      </c>
-      <c r="J677" t="n">
-        <v>0</v>
-      </c>
-      <c r="K677" t="n">
-        <v>0</v>
-      </c>
-      <c r="L677" t="n">
-        <v>0</v>
-      </c>
-      <c r="M677" t="n">
-        <v>0</v>
-      </c>
-      <c r="N677" t="n">
-        <v>0</v>
-      </c>
-      <c r="O677" t="n">
+      <c r="E684" t="n">
+        <v>0</v>
+      </c>
+      <c r="F684" t="n">
+        <v>0</v>
+      </c>
+      <c r="G684" t="n">
+        <v>0</v>
+      </c>
+      <c r="H684" t="n">
+        <v>0</v>
+      </c>
+      <c r="I684" t="n">
+        <v>0</v>
+      </c>
+      <c r="J684" t="n">
+        <v>0</v>
+      </c>
+      <c r="K684" t="n">
+        <v>0</v>
+      </c>
+      <c r="L684" t="n">
+        <v>0</v>
+      </c>
+      <c r="M684" t="n">
+        <v>0</v>
+      </c>
+      <c r="N684" t="n">
+        <v>0</v>
+      </c>
+      <c r="O684" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>